<commit_message>
Update test_data for pro_gripper
</commit_message>
<xml_diff>
--- a/test_data/test_mercury.xlsx
+++ b/test_data/test_mercury.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10500" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="28800" windowHeight="12300" firstSheet="14" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="get_modified_version" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,20 @@
     <sheet name="get_robot_type" sheetId="5" r:id="rId5"/>
     <sheet name="get_limit_switch" sheetId="6" r:id="rId6"/>
     <sheet name="clear_error_information" sheetId="7" r:id="rId7"/>
+    <sheet name="power_on" sheetId="8" r:id="rId8"/>
+    <sheet name="power_off" sheetId="9" r:id="rId9"/>
+    <sheet name="is_power_on" sheetId="10" r:id="rId10"/>
+    <sheet name="power_on_only" sheetId="11" r:id="rId11"/>
+    <sheet name="set_servo_calibration" sheetId="12" r:id="rId12"/>
+    <sheet name="get_joint_max_angle" sheetId="13" r:id="rId13"/>
+    <sheet name="get_joint_min_angle" sheetId="14" r:id="rId14"/>
+    <sheet name="set_joint_max_angle" sheetId="15" r:id="rId15"/>
+    <sheet name="set_joint_min_angle" sheetId="16" r:id="rId16"/>
+    <sheet name="get_robot_status" sheetId="17" r:id="rId17"/>
+    <sheet name="over_limit_return_zero" sheetId="18" r:id="rId18"/>
+    <sheet name="get_angle" sheetId="19" r:id="rId19"/>
+    <sheet name="get_model_direction" sheetId="20" r:id="rId20"/>
+    <sheet name="get_movement_type" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -123,6 +137,249 @@
   </si>
   <si>
     <t>clear_error_information</t>
+  </si>
+  <si>
+    <t>机械臂正常上电</t>
+  </si>
+  <si>
+    <t>power_on</t>
+  </si>
+  <si>
+    <t>机械臂正常下电</t>
+  </si>
+  <si>
+    <t>power_off</t>
+  </si>
+  <si>
+    <t>test_type</t>
+  </si>
+  <si>
+    <t>检查机械臂上电状态下返回</t>
+  </si>
+  <si>
+    <t>is_power_on</t>
+  </si>
+  <si>
+    <t>检查机械臂下电状态下返回</t>
+  </si>
+  <si>
+    <t>检查机械臂power_on_only状态下返回</t>
+  </si>
+  <si>
+    <t>机械臂正常仅上电</t>
+  </si>
+  <si>
+    <t>power_on_only</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>设置1关节零位</t>
+  </si>
+  <si>
+    <t>set_servo_Calibration</t>
+  </si>
+  <si>
+    <t>设置2关节零位</t>
+  </si>
+  <si>
+    <t>设置3关节零位</t>
+  </si>
+  <si>
+    <t>设置4关节零位</t>
+  </si>
+  <si>
+    <t>设置5关节零位</t>
+  </si>
+  <si>
+    <t>设置6关节零位</t>
+  </si>
+  <si>
+    <t>设置7关节零位</t>
+  </si>
+  <si>
+    <t>设置关节零位（超限）</t>
+  </si>
+  <si>
+    <t>正确获取1关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>get_joint_max_angle</t>
+  </si>
+  <si>
+    <t>normal</t>
+  </si>
+  <si>
+    <t>正确获取2关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确获取3关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确获取4关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确获取5关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确获取6关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确获取7关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>获取关节软件限位最大值（超限）</t>
+  </si>
+  <si>
+    <t>exception</t>
+  </si>
+  <si>
+    <t>正确获取1关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>get_joint_min_angle</t>
+  </si>
+  <si>
+    <t>正确获取2关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确获取3关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确获取4关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确获取5关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确获取6关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确获取7关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>获取关节软件限位最小值（超限）</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>正确设置1关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>set_joint_max_angle</t>
+  </si>
+  <si>
+    <t>正确设置2关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确设置3关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确设置4关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确设置5关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确设置6关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>正确设置7关节软件限位最大值</t>
+  </si>
+  <si>
+    <t>设置关节软件限位最大值关节（超限）</t>
+  </si>
+  <si>
+    <t>设置关节软件限位最大值（超限）</t>
+  </si>
+  <si>
+    <t>正确设置1关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>set_joint_min_angle</t>
+  </si>
+  <si>
+    <t>正确设置2关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确设置3关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确设置4关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确设置5关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确设置6关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>正确设置7关节软件限位最小值</t>
+  </si>
+  <si>
+    <t>设置关节软件限位最小值关节（超限）</t>
+  </si>
+  <si>
+    <t>设置关节软件限位最小值（超限）</t>
+  </si>
+  <si>
+    <t>获取机械臂状态</t>
+  </si>
+  <si>
+    <t>get_robot_status</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,0,0]</t>
+  </si>
+  <si>
+    <t>机械臂回到零位</t>
+  </si>
+  <si>
+    <t>over_limit_return_zero</t>
+  </si>
+  <si>
+    <t>set_angle</t>
+  </si>
+  <si>
+    <t>正确获取1关节角度</t>
+  </si>
+  <si>
+    <t>get_angle</t>
+  </si>
+  <si>
+    <t>正确获取2关节角度</t>
+  </si>
+  <si>
+    <t>正确获取3关节角度</t>
+  </si>
+  <si>
+    <t>正确获取4关节角度</t>
+  </si>
+  <si>
+    <t>正确获取5关节角度</t>
+  </si>
+  <si>
+    <t>正确获取6关节角度</t>
+  </si>
+  <si>
+    <t>正确获取7关节角度</t>
+  </si>
+  <si>
+    <t>获取关节角度关节（超限）</t>
+  </si>
+  <si>
+    <t>正确获取关节模型方向</t>
+  </si>
+  <si>
+    <t>get_model_direction</t>
+  </si>
+  <si>
+    <t>正确获取机械臂运动模式</t>
+  </si>
+  <si>
+    <t>get_movement_type</t>
   </si>
 </sst>
 </file>
@@ -738,18 +995,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1113,53 +1367,53 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="3" width="9" style="3"/>
-    <col min="4" max="4" width="56.8796296296296" style="3" customWidth="1"/>
-    <col min="5" max="6" width="19" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="3"/>
+    <col min="1" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="56.8796296296296" style="1" customWidth="1"/>
+    <col min="5" max="6" width="19" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="48" customHeight="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="90" customHeight="1" spans="1:7">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>4</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <v>4</v>
       </c>
     </row>
@@ -1173,134 +1427,2084 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.6666666666667" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="28.8" spans="1:7">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" ht="43.2" spans="1:7">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="28.8" spans="1:6">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="28.8" spans="1:6">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="28.8" spans="1:6">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="28.8" spans="1:6">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="28.8" spans="1:6">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="28.8" spans="1:6">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="28.8" spans="1:4">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" ht="28.8" spans="1:4">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>165</v>
+      </c>
+      <c r="F2" s="1">
+        <v>165</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>120</v>
+      </c>
+      <c r="F3" s="1">
+        <v>120</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>165</v>
+      </c>
+      <c r="F4" s="1">
+        <v>165</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>165</v>
+      </c>
+      <c r="F6" s="1">
+        <v>165</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>265</v>
+      </c>
+      <c r="F7" s="1">
+        <v>265</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>180</v>
+      </c>
+      <c r="F8" s="1">
+        <v>180</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="43.2" spans="1:7">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="43.2" spans="1:7">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:7">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-165</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-165</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-50</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-50</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-165</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-165</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-165</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-165</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-165</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-165</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-20</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="28.8" spans="1:7">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-180</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-180</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="43.2" spans="1:7">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="43.2" spans="1:7">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>160</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>110</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>150</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>140</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>250</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>170</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="43.2" spans="1:8">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="43.2" spans="1:8">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" ht="43.2" spans="1:8">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>180</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-150</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-40</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-140</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-155</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-160</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-15</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-175</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="43.2" spans="1:8">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="43.2" spans="1:8">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" ht="43.2" spans="1:8">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>180</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="17.6666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1111111111111" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.3333333333333" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="17.6666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1111111111111" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="14.6666666666667" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" ht="28.8" spans="1:8">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="13.2222222222222" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1111111111111" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.6666666666667" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.3333333333333" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="3"/>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6666666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.3333333333333" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:8">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="28.8" spans="1:8">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="43.2" spans="1:6">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" ht="43.2" spans="1:6">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.3333333333333" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1316,52 +3520,52 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.2222222222222" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.2222222222222" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.1111111111111" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:7">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>1.2</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <v>1.2</v>
       </c>
     </row>
@@ -1383,52 +3587,52 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.2222222222222" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.2222222222222" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.1111111111111" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:7">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>1.1</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="1">
         <v>1.1</v>
       </c>
     </row>
@@ -1449,7 +3653,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.2222222222222" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.2222222222222" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.1111111111111" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="16.5555555555556" customWidth="1"/>
@@ -1457,46 +3661,46 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:7">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>4501</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>4502</v>
       </c>
     </row>
@@ -1517,52 +3721,52 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.2222222222222" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.2222222222222" style="3" customWidth="1"/>
     <col min="2" max="2" width="16.1111111111111" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1577,53 +3781,173 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="13.2222222222222" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1111111111111" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="28.8" spans="1:6">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.2222222222222" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.1111111111111" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="28.8" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="30" customHeight="1" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>